<commit_message>
I ran 4 tests
I ran 4 tests: 4 tests were launched, all tests passed
</commit_message>
<xml_diff>
--- a/Tests vk.xlsx
+++ b/Tests vk.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="146">
   <si>
     <t xml:space="preserve">passed</t>
   </si>
@@ -2009,7 +2009,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="7" topLeftCell="L8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M8" activeCellId="0" sqref="M8"/>
+      <selection pane="bottomLeft" activeCell="L11" activeCellId="0" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2098,7 +2098,7 @@
       <c r="K2" s="6"/>
       <c r="L2" s="9" t="n">
         <f aca="false">COUNTIF(L$8:L$39,"passed")</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M2" s="6"/>
       <c r="N2" s="9" t="n">
@@ -2361,7 +2361,9 @@
       <c r="I9" s="29"/>
       <c r="J9" s="23"/>
       <c r="K9" s="25"/>
-      <c r="L9" s="26"/>
+      <c r="L9" s="26" t="s">
+        <v>0</v>
+      </c>
       <c r="M9" s="6"/>
       <c r="N9" s="26"/>
       <c r="O9" s="6"/>
@@ -2397,7 +2399,9 @@
       <c r="I10" s="24"/>
       <c r="J10" s="23"/>
       <c r="K10" s="25"/>
-      <c r="L10" s="26"/>
+      <c r="L10" s="26" t="s">
+        <v>0</v>
+      </c>
       <c r="M10" s="6"/>
       <c r="N10" s="26"/>
       <c r="O10" s="6"/>
@@ -2433,7 +2437,9 @@
       <c r="I11" s="24"/>
       <c r="J11" s="23"/>
       <c r="K11" s="25"/>
-      <c r="L11" s="26"/>
+      <c r="L11" s="26" t="s">
+        <v>0</v>
+      </c>
       <c r="M11" s="6"/>
       <c r="N11" s="26"/>
       <c r="O11" s="6"/>

</xml_diff>